<commit_message>
fix testing all test case
</commit_message>
<xml_diff>
--- a/cypress/downloads/most_borrowed_books.xlsx
+++ b/cypress/downloads/most_borrowed_books.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,51 +415,18 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>5107068454</v>
+        <v>2663854991</v>
       </c>
       <c r="B2" t="str">
-        <v>Veritatis sint maiores aut.</v>
+        <v>Quia aut autem.</v>
       </c>
       <c r="C2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2663854991</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Quia aut autem.</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>1393227084</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Officiis distinctio et esse.</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2748540941</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Beatae possimus quia.</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>